<commit_message>
corretto valore workflowinstanceId quando non valorizzato
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#HEALTHTELEMATICNETWORKSRLXX/Health_Telematic_Network_S.r.l./HTN_Virtual_Hospital/3.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#HEALTHTELEMATICNETWORKSRLXX/Health_Telematic_Network_S.r.l./HTN_Virtual_Hospital/3.0/report-checklist.xlsx
@@ -338,7 +338,7 @@
     <t>5f8d2048bda87e63d0339b224c3abdd2</t>
   </si>
   <si>
-    <t>UNKNOWN_WORKFLOW_ID</t>
+    <t/>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CERT_VAC_KO</t>
@@ -2148,7 +2148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -2256,6 +2256,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2625,35 +2628,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="49" width="130.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="50" width="130.14785714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>474</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25" customFormat="1" s="20">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="67.5" customFormat="1" s="20">
       <c r="A2" s="11" t="s">
         <v>475</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25" customFormat="1" s="20">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="40.5" customFormat="1" s="20">
       <c r="A3" s="11" t="s">
         <v>476</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25" customFormat="1" s="20">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="77.25" customFormat="1" s="20">
       <c r="A4" s="11" t="s">
         <v>477</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25" customFormat="1" s="20">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="293.25" customFormat="1" s="20">
       <c r="A5" s="11" t="s">
         <v>478</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25" customFormat="1" s="20">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="4.5" customFormat="1" s="20">
       <c r="A6" s="11" t="s">
         <v>479</v>
       </c>
@@ -2667,7 +2670,7 @@
       <c r="A8" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="49" t="s">
         <v>481</v>
       </c>
     </row>
@@ -2703,13 +2706,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="37" width="3.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="38" width="3.1478571428571427" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="194.14785714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="14.25" customFormat="1" s="20">
-      <c r="A1" s="40"/>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="41"/>
+      <c r="B1" s="42" t="s">
         <v>466</v>
       </c>
     </row>
@@ -2724,50 +2727,50 @@
       <c r="B3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="14.25">
-      <c r="A4" s="42">
+      <c r="A4" s="43">
         <v>1</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="44" t="s">
         <v>468</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="14.25">
-      <c r="A5" s="44">
+      <c r="A5" s="45">
         <v>2</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="46" t="s">
         <v>469</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="14.25">
-      <c r="A6" s="44">
+      <c r="A6" s="45">
         <v>3</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="46" t="s">
         <v>470</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="14.25">
-      <c r="A7" s="44">
+      <c r="A7" s="45">
         <v>4</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="46" t="s">
         <v>471</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="30">
-      <c r="A8" s="44">
+      <c r="A8" s="45">
         <v>5</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="46" t="s">
         <v>472</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="14.25">
-      <c r="A9" s="46">
+      <c r="A9" s="47">
         <v>6</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="48" t="s">
         <v>473</v>
       </c>
     </row>
@@ -6737,11 +6740,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="37" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="38" width="10.719285714285713" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1" hidden="1"/>
-    <col min="3" max="3" style="38" width="12.43357142857143" customWidth="1" bestFit="1" hidden="1"/>
+    <col min="3" max="3" style="39" width="12.43357142857143" customWidth="1" bestFit="1" hidden="1"/>
     <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1" hidden="1"/>
-    <col min="5" max="5" style="39" width="12.43357142857143" customWidth="1" bestFit="1" hidden="1"/>
+    <col min="5" max="5" style="40" width="12.43357142857143" customWidth="1" bestFit="1" hidden="1"/>
     <col min="6" max="6" style="2" width="12.43357142857143" customWidth="1" bestFit="1" hidden="1"/>
     <col min="7" max="7" style="2" width="33.14785714285715" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="2" width="33.14785714285715" customWidth="1" bestFit="1"/>
@@ -6757,7 +6760,7 @@
     <col min="18" max="18" style="2" width="36.43357142857143" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="2" width="27.14785714285714" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="2" width="33.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="37" width="36.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="38" width="36.43357142857143" customWidth="1" bestFit="1"/>
     <col min="22" max="22" style="2" width="31.862142857142857" customWidth="1" bestFit="1"/>
     <col min="23" max="23" style="2" width="31.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
@@ -6974,7 +6977,7 @@
       <c r="V8" s="11"/>
       <c r="W8" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="25.5" customFormat="1" s="20">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="101.25" customFormat="1" s="20">
       <c r="A9" s="21" t="s">
         <v>55</v>
       </c>
@@ -7255,7 +7258,7 @@
       <c r="H15" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="36" t="s">
+      <c r="I15" s="37" t="s">
         <v>87</v>
       </c>
       <c r="J15" s="32" t="s">
@@ -7561,7 +7564,7 @@
       <c r="H23" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="I23" s="36" t="s">
+      <c r="I23" s="37" t="s">
         <v>87</v>
       </c>
       <c r="J23" s="32" t="s">
@@ -28156,7 +28159,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="70.7192857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">

</xml_diff>